<commit_message>
Add SHAP for Feature Importance; remove SOFA resp
</commit_message>
<xml_diff>
--- a/results/xgb_results.xlsx
+++ b/results/xgb_results.xlsx
@@ -472,22 +472,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>65213</v>
+        <v>16124</v>
       </c>
       <c r="C2" t="n">
-        <v>43960</v>
+        <v>10961</v>
       </c>
       <c r="D2" t="n">
-        <v>2355</v>
+        <v>451</v>
       </c>
       <c r="E2" t="n">
-        <v>2032</v>
+        <v>189</v>
       </c>
       <c r="F2" t="n">
-        <v>12283</v>
+        <v>3512</v>
       </c>
       <c r="G2" t="n">
-        <v>4583</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.2577258571781198</v>
+        <v>-0.1447299462922762</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.2592933801996105</v>
+        <v>-0.1492223798200119</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.4304899984922121</v>
+        <v>-0.07536776923588184</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.418267336150709</v>
+        <v>0.2185821020819343</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2022321904020647</v>
+        <v>-0.2456433932824857</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.3117379043898987</v>
+        <v>0.06028432561899122</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.2588068420145428</v>
+        <v>-0.1485768202172113</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.2608996583421332</v>
+        <v>-0.1549126428413103</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4653496329202207</v>
+        <v>-0.2220088286771384</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.4584814985934633</v>
+        <v>-0.09631764782534602</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2077388976376704</v>
+        <v>-0.2651009412249949</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.3279679800960043</v>
+        <v>0.00720415154307652</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.633944766688242</v>
+        <v>3.369940413048412</v>
       </c>
       <c r="C5" t="n">
-        <v>3.487389279309282</v>
+        <v>3.386813866351882</v>
       </c>
       <c r="D5" t="n">
-        <v>3.719386863609238</v>
+        <v>2.76339711883103</v>
       </c>
       <c r="E5" t="n">
-        <v>3.925869430763277</v>
+        <v>2.701165729142938</v>
       </c>
       <c r="F5" t="n">
-        <v>3.855165251009954</v>
+        <v>3.388435041038097</v>
       </c>
       <c r="G5" t="n">
-        <v>4.180286852255408</v>
+        <v>3.479193489771451</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1140</v>
+        <v>240</v>
       </c>
       <c r="C6" t="n">
-        <v>662</v>
+        <v>165</v>
       </c>
       <c r="D6" t="n">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="G6" t="n">
-        <v>137</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -597,22 +597,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7145551713095761</v>
+        <v>0.2968447583444246</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6896255325973231</v>
+        <v>0.2850602023802188</v>
       </c>
       <c r="D7" t="n">
-        <v>0.696850960714531</v>
+        <v>0.3847566437620272</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7335878464687542</v>
+        <v>0.435241139923141</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7586992719203978</v>
+        <v>0.2845470015691641</v>
       </c>
       <c r="G7" t="n">
-        <v>0.7666271894709605</v>
+        <v>0.3754272205442577</v>
       </c>
     </row>
     <row r="8">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.7143098384099711</v>
+        <v>0.29448179966315</v>
       </c>
       <c r="C8" t="n">
-        <v>0.689229637779781</v>
+        <v>0.281520247394755</v>
       </c>
       <c r="D8" t="n">
-        <v>0.689463516763275</v>
+        <v>0.3008598224568491</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7260338816091341</v>
+        <v>0.2076517485488844</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7575940174812961</v>
+        <v>0.2733712821837823</v>
       </c>
       <c r="G8" t="n">
-        <v>0.7637396778957006</v>
+        <v>0.3401480049683058</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.731196705755877</v>
+        <v>2.641169716150813</v>
       </c>
       <c r="C9" t="n">
-        <v>1.731330427279378</v>
+        <v>2.671308390905421</v>
       </c>
       <c r="D9" t="n">
-        <v>1.712210035306577</v>
+        <v>2.090201999751256</v>
       </c>
       <c r="E9" t="n">
-        <v>1.701507303510631</v>
+        <v>2.296365853398741</v>
       </c>
       <c r="F9" t="n">
-        <v>1.72714237168156</v>
+        <v>2.5679871953144</v>
       </c>
       <c r="G9" t="n">
-        <v>1.76322477030246</v>
+        <v>2.836428711636537</v>
       </c>
     </row>
     <row r="10">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>747</v>
+        <v>339</v>
       </c>
       <c r="C10" t="n">
-        <v>477</v>
+        <v>228</v>
       </c>
       <c r="D10" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E10" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="G10" t="n">
-        <v>75</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9722810284876959</v>
+        <v>0.4415747046367008</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9489189127969335</v>
+        <v>0.4342825822002306</v>
       </c>
       <c r="D11" t="n">
-        <v>1.127340959206743</v>
+        <v>0.4601244129979091</v>
       </c>
       <c r="E11" t="n">
-        <v>1.151855182619463</v>
+        <v>0.2166590378412067</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9609314623224625</v>
+        <v>0.5301903948516499</v>
       </c>
       <c r="G11" t="n">
-        <v>1.078365093860859</v>
+        <v>0.3151428949252665</v>
       </c>
     </row>
     <row r="12">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9731166804245139</v>
+        <v>0.4430586198803613</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9501292961219142</v>
+        <v>0.4364328902360654</v>
       </c>
       <c r="D12" t="n">
-        <v>1.154813149683496</v>
+        <v>0.5228686511339875</v>
       </c>
       <c r="E12" t="n">
-        <v>1.184515380202597</v>
+        <v>0.3039693963742304</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9653329151189665</v>
+        <v>0.5384722234087772</v>
       </c>
       <c r="G12" t="n">
-        <v>1.091707657991705</v>
+        <v>0.3329438534252293</v>
       </c>
     </row>
     <row r="13">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.902748060932366</v>
+        <v>0.7287706968975982</v>
       </c>
       <c r="C13" t="n">
-        <v>1.756058852029903</v>
+        <v>0.7155054754464607</v>
       </c>
       <c r="D13" t="n">
-        <v>2.007176828302661</v>
+        <v>0.6731951190797734</v>
       </c>
       <c r="E13" t="n">
-        <v>2.224362127252645</v>
+        <v>0.4047998757441964</v>
       </c>
       <c r="F13" t="n">
-        <v>2.128022879328394</v>
+        <v>0.820447845723697</v>
       </c>
       <c r="G13" t="n">
-        <v>2.417062081952948</v>
+        <v>0.6427647781349139</v>
       </c>
     </row>
     <row r="14">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>393</v>
+        <v>-99</v>
       </c>
       <c r="C14" t="n">
-        <v>185</v>
+        <v>-63</v>
       </c>
       <c r="D14" t="n">
-        <v>9</v>
+        <v>-3</v>
       </c>
       <c r="E14" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>121</v>
+        <v>-20</v>
       </c>
       <c r="G14" t="n">
-        <v>62</v>
+        <v>-13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add multi-task regression (doesn't work)
</commit_message>
<xml_diff>
--- a/results/xgb_results.xlsx
+++ b/results/xgb_results.xlsx
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1485768202172113</v>
+        <v>-0.14871979361862</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1549126428413103</v>
+        <v>-0.1551244756811565</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2220088286771384</v>
+        <v>-0.2282119191780376</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.09631764782534602</v>
+        <v>-0.1129285212772451</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2651009412249949</v>
+        <v>-0.2658332717264276</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00720415154307652</v>
+        <v>0.005122818527443562</v>
       </c>
     </row>
     <row r="5">
@@ -597,22 +597,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2968447583444246</v>
+        <v>0.4478752838460561</v>
       </c>
       <c r="C7" t="n">
-        <v>0.2850602023802188</v>
+        <v>0.4346435041987016</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3847566437620272</v>
+        <v>0.5641682672869548</v>
       </c>
       <c r="E7" t="n">
-        <v>0.435241139923141</v>
+        <v>0.6330952554014504</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2845470015691641</v>
+        <v>0.4476816913065088</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3754272205442577</v>
+        <v>0.4974829832875998</v>
       </c>
     </row>
     <row r="8">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.29448179966315</v>
+        <v>0.4459509056731166</v>
       </c>
       <c r="C8" t="n">
-        <v>0.281520247394755</v>
+        <v>0.431739985878372</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3008598224568491</v>
+        <v>0.5022226403023595</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2076517485488844</v>
+        <v>0.4774386970869142</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2733712821837823</v>
+        <v>0.4387294987488141</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3401480049683058</v>
+        <v>0.4679851290571024</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.641169716150813</v>
+        <v>2.340395714487467</v>
       </c>
       <c r="C9" t="n">
-        <v>2.671308390905421</v>
+        <v>2.37547511409402</v>
       </c>
       <c r="D9" t="n">
-        <v>2.090201999751256</v>
+        <v>1.759236457395349</v>
       </c>
       <c r="E9" t="n">
-        <v>2.296365853398741</v>
+        <v>1.850913903771682</v>
       </c>
       <c r="F9" t="n">
-        <v>2.5679871953144</v>
+        <v>2.256300916109789</v>
       </c>
       <c r="G9" t="n">
-        <v>2.836428711636537</v>
+        <v>2.544226272518651</v>
       </c>
     </row>
     <row r="10">
@@ -672,122 +672,122 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>339</v>
+        <v>275</v>
       </c>
       <c r="C10" t="n">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" t="n">
         <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="G10" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Lift R²</t>
+          <t>Delta R²</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4415747046367008</v>
+        <v>0.5926052301383323</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4342825822002306</v>
+        <v>0.5838658840187134</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4601244129979091</v>
+        <v>0.6395360365228366</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2166590378412067</v>
+        <v>0.4145131533195161</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5301903948516499</v>
+        <v>0.6933250845889946</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3151428949252665</v>
+        <v>0.4371986576686085</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Lift Adj R²</t>
+          <t>Delta Adj R²</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4430586198803613</v>
+        <v>0.5946706992917365</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4364328902360654</v>
+        <v>0.5868644615595285</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5228686511339875</v>
+        <v>0.7304345594803971</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3039693963742304</v>
+        <v>0.5903672183641593</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5384722234087772</v>
+        <v>0.7045627704752416</v>
       </c>
       <c r="G12" t="n">
-        <v>0.3329438534252293</v>
+        <v>0.4628623105296589</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Drop RMSE</t>
+          <t>Delta RMSE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.7287706968975982</v>
+        <v>-1.029544698560945</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7155054754464607</v>
+        <v>-1.011338752257862</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6731951190797734</v>
+        <v>-1.004160661435681</v>
       </c>
       <c r="E13" t="n">
-        <v>0.4047998757441964</v>
+        <v>-0.8502518253712559</v>
       </c>
       <c r="F13" t="n">
-        <v>0.820447845723697</v>
+        <v>-1.132134124928308</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6427647781349139</v>
+        <v>-0.9349672172528005</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Drop HH</t>
+          <t>Delta HH</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-99</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>-63</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>-20</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>-13</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add XGBoost Classifier for Hidden Hypoxemias; Interaction Variables and Deltas
</commit_message>
<xml_diff>
--- a/results/xgb_results.xlsx
+++ b/results/xgb_results.xlsx
@@ -472,22 +472,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16124</v>
+        <v>4076</v>
       </c>
       <c r="C2" t="n">
-        <v>10961</v>
+        <v>2763</v>
       </c>
       <c r="D2" t="n">
-        <v>451</v>
+        <v>131</v>
       </c>
       <c r="E2" t="n">
-        <v>189</v>
+        <v>110</v>
       </c>
       <c r="F2" t="n">
-        <v>3512</v>
+        <v>816</v>
       </c>
       <c r="G2" t="n">
-        <v>1011</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1447299462922762</v>
+        <v>-0.01052456029596116</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1492223798200119</v>
+        <v>-0.0321981526640378</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.07536776923588184</v>
+        <v>-0.05707477054479404</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2185821020819343</v>
+        <v>-0.6687957480535223</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.2456433932824857</v>
+        <v>-0.001651116592686241</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06028432561899122</v>
+        <v>0.313326173972469</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.14871979361862</v>
+        <v>-0.03542559296103653</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.1551244756811565</v>
+        <v>-0.07016940602780486</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2282119191780376</v>
+        <v>-3.294366255338225</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1129285212772451</v>
+        <v>-15.53624877616672</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2658332717264276</v>
+        <v>-0.1385574058898735</v>
       </c>
       <c r="G4" t="n">
-        <v>0.005122818527443562</v>
+        <v>-0.1152982524650981</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.369940413048412</v>
+        <v>3.436401711423847</v>
       </c>
       <c r="C5" t="n">
-        <v>3.386813866351882</v>
+        <v>3.3612301705088</v>
       </c>
       <c r="D5" t="n">
-        <v>2.76339711883103</v>
+        <v>3.231524112799261</v>
       </c>
       <c r="E5" t="n">
-        <v>2.701165729142938</v>
+        <v>3.845895096191404</v>
       </c>
       <c r="F5" t="n">
-        <v>3.388435041038097</v>
+        <v>3.790450138822823</v>
       </c>
       <c r="G5" t="n">
-        <v>3.479193489771451</v>
+        <v>2.93017704243276</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>240</v>
+        <v>74</v>
       </c>
       <c r="C6" t="n">
-        <v>165</v>
+        <v>47</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="G6" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -597,22 +597,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4478752838460561</v>
+        <v>0.4960832566928129</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4346435041987016</v>
+        <v>0.4341680724834786</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5641682672869548</v>
+        <v>0.5428263380630094</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6330952554014504</v>
+        <v>0.2316452809869561</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4476816913065088</v>
+        <v>0.6121035607998226</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4974829832875998</v>
+        <v>0.6846531514767573</v>
       </c>
     </row>
     <row r="8">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4459509056731166</v>
+        <v>0.4836658966616074</v>
       </c>
       <c r="C8" t="n">
-        <v>0.431739985878372</v>
+        <v>0.4133529340087717</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5022226403023595</v>
+        <v>-0.8572680016190244</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4774386970869142</v>
+        <v>-6.613696761129253</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4387294987488141</v>
+        <v>0.5590856374502866</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4679851290571024</v>
+        <v>0.4878124434813574</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.340395714487467</v>
+        <v>2.426665324080497</v>
       </c>
       <c r="C9" t="n">
-        <v>2.37547511409402</v>
+        <v>2.488630612230798</v>
       </c>
       <c r="D9" t="n">
-        <v>1.759236457395349</v>
+        <v>2.125177201954327</v>
       </c>
       <c r="E9" t="n">
-        <v>1.850913903771682</v>
+        <v>2.609616700909467</v>
       </c>
       <c r="F9" t="n">
-        <v>2.256300916109789</v>
+        <v>2.358796337740918</v>
       </c>
       <c r="G9" t="n">
-        <v>2.544226272518651</v>
+        <v>1.985696462501479</v>
       </c>
     </row>
     <row r="10">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>275</v>
+        <v>72</v>
       </c>
       <c r="C10" t="n">
-        <v>190</v>
+        <v>48</v>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="G10" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5926052301383323</v>
+        <v>0.5066078169887741</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5838658840187134</v>
+        <v>0.4663662251475164</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6395360365228366</v>
+        <v>0.5999011086078034</v>
       </c>
       <c r="E11" t="n">
-        <v>0.4145131533195161</v>
+        <v>0.9004410290404784</v>
       </c>
       <c r="F11" t="n">
-        <v>0.6933250845889946</v>
+        <v>0.6137546773925089</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4371986576686085</v>
+        <v>0.3713269775042883</v>
       </c>
     </row>
     <row r="12">
@@ -722,22 +722,22 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5946706992917365</v>
+        <v>0.519091489622644</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5868644615595285</v>
+        <v>0.4835223400365766</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7304345594803971</v>
+        <v>2.437098253719201</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5903672183641593</v>
+        <v>8.92255201503747</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7045627704752416</v>
+        <v>0.6976430433401601</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4628623105296589</v>
+        <v>0.6031106959464555</v>
       </c>
     </row>
     <row r="13">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1.029544698560945</v>
+        <v>-1.00973638734335</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.011338752257862</v>
+        <v>-0.8725995582780022</v>
       </c>
       <c r="D13" t="n">
-        <v>-1.004160661435681</v>
+        <v>-1.106346910844934</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.8502518253712559</v>
+        <v>-1.236278395281937</v>
       </c>
       <c r="F13" t="n">
-        <v>-1.132134124928308</v>
+        <v>-1.431653801081905</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.9349672172528005</v>
+        <v>-0.9444805799312816</v>
       </c>
     </row>
     <row r="14">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>35</v>
+        <v>-2</v>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="G14" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>